<commit_message>
first epoch run on EC2
fourth epoch run on EC2. training and validation files rebuilt. accuracy reached 75%. small reorg of global variables to accomodate running validation directly.
</commit_message>
<xml_diff>
--- a/Training results.xlsx
+++ b/Training results.xlsx
@@ -16,7 +16,7 @@
     <sheet name="batch256" sheetId="1" r:id="rId2"/>
     <sheet name="batch128" sheetId="2" r:id="rId3"/>
     <sheet name="keep.7" sheetId="4" r:id="rId4"/>
-    <sheet name="keep.7ep2" sheetId="5" r:id="rId5"/>
+    <sheet name="keep.7ep4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -4647,7 +4647,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>30% Dropout 3 Epochs</c:v>
+            <c:v>30% Dropout 4 Epochs</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -4679,7 +4679,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>keep.7ep2!$F:$F</c:f>
+              <c:f>keep.7ep4!$F:$F</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
@@ -7725,12 +7725,1023 @@
                 <c:pt idx="1013">
                   <c:v>12946</c:v>
                 </c:pt>
+                <c:pt idx="1014">
+                  <c:v>12958</c:v>
+                </c:pt>
+                <c:pt idx="1015">
+                  <c:v>12971</c:v>
+                </c:pt>
+                <c:pt idx="1016">
+                  <c:v>12984</c:v>
+                </c:pt>
+                <c:pt idx="1017">
+                  <c:v>12997</c:v>
+                </c:pt>
+                <c:pt idx="1018">
+                  <c:v>13010</c:v>
+                </c:pt>
+                <c:pt idx="1019">
+                  <c:v>13022</c:v>
+                </c:pt>
+                <c:pt idx="1020">
+                  <c:v>13035</c:v>
+                </c:pt>
+                <c:pt idx="1021">
+                  <c:v>13048</c:v>
+                </c:pt>
+                <c:pt idx="1022">
+                  <c:v>13061</c:v>
+                </c:pt>
+                <c:pt idx="1023">
+                  <c:v>13074</c:v>
+                </c:pt>
+                <c:pt idx="1024">
+                  <c:v>13086</c:v>
+                </c:pt>
+                <c:pt idx="1025">
+                  <c:v>13099</c:v>
+                </c:pt>
+                <c:pt idx="1026">
+                  <c:v>13112</c:v>
+                </c:pt>
+                <c:pt idx="1027">
+                  <c:v>13125</c:v>
+                </c:pt>
+                <c:pt idx="1028">
+                  <c:v>13138</c:v>
+                </c:pt>
+                <c:pt idx="1029">
+                  <c:v>13150</c:v>
+                </c:pt>
+                <c:pt idx="1030">
+                  <c:v>13163</c:v>
+                </c:pt>
+                <c:pt idx="1031">
+                  <c:v>13176</c:v>
+                </c:pt>
+                <c:pt idx="1032">
+                  <c:v>13189</c:v>
+                </c:pt>
+                <c:pt idx="1033">
+                  <c:v>13202</c:v>
+                </c:pt>
+                <c:pt idx="1034">
+                  <c:v>13214</c:v>
+                </c:pt>
+                <c:pt idx="1035">
+                  <c:v>13227</c:v>
+                </c:pt>
+                <c:pt idx="1036">
+                  <c:v>13240</c:v>
+                </c:pt>
+                <c:pt idx="1037">
+                  <c:v>13253</c:v>
+                </c:pt>
+                <c:pt idx="1038">
+                  <c:v>13266</c:v>
+                </c:pt>
+                <c:pt idx="1039">
+                  <c:v>13278</c:v>
+                </c:pt>
+                <c:pt idx="1040">
+                  <c:v>13291</c:v>
+                </c:pt>
+                <c:pt idx="1041">
+                  <c:v>13304</c:v>
+                </c:pt>
+                <c:pt idx="1042">
+                  <c:v>13317</c:v>
+                </c:pt>
+                <c:pt idx="1043">
+                  <c:v>13330</c:v>
+                </c:pt>
+                <c:pt idx="1044">
+                  <c:v>13342</c:v>
+                </c:pt>
+                <c:pt idx="1045">
+                  <c:v>13355</c:v>
+                </c:pt>
+                <c:pt idx="1046">
+                  <c:v>13368</c:v>
+                </c:pt>
+                <c:pt idx="1047">
+                  <c:v>13381</c:v>
+                </c:pt>
+                <c:pt idx="1048">
+                  <c:v>13394</c:v>
+                </c:pt>
+                <c:pt idx="1049">
+                  <c:v>13406</c:v>
+                </c:pt>
+                <c:pt idx="1050">
+                  <c:v>13419</c:v>
+                </c:pt>
+                <c:pt idx="1051">
+                  <c:v>13432</c:v>
+                </c:pt>
+                <c:pt idx="1052">
+                  <c:v>13445</c:v>
+                </c:pt>
+                <c:pt idx="1053">
+                  <c:v>13458</c:v>
+                </c:pt>
+                <c:pt idx="1054">
+                  <c:v>13470</c:v>
+                </c:pt>
+                <c:pt idx="1055">
+                  <c:v>13483</c:v>
+                </c:pt>
+                <c:pt idx="1056">
+                  <c:v>13496</c:v>
+                </c:pt>
+                <c:pt idx="1057">
+                  <c:v>13509</c:v>
+                </c:pt>
+                <c:pt idx="1058">
+                  <c:v>13522</c:v>
+                </c:pt>
+                <c:pt idx="1059">
+                  <c:v>13534</c:v>
+                </c:pt>
+                <c:pt idx="1060">
+                  <c:v>13547</c:v>
+                </c:pt>
+                <c:pt idx="1061">
+                  <c:v>13560</c:v>
+                </c:pt>
+                <c:pt idx="1062">
+                  <c:v>13573</c:v>
+                </c:pt>
+                <c:pt idx="1063">
+                  <c:v>13586</c:v>
+                </c:pt>
+                <c:pt idx="1064">
+                  <c:v>13598</c:v>
+                </c:pt>
+                <c:pt idx="1065">
+                  <c:v>13611</c:v>
+                </c:pt>
+                <c:pt idx="1066">
+                  <c:v>13624</c:v>
+                </c:pt>
+                <c:pt idx="1067">
+                  <c:v>13637</c:v>
+                </c:pt>
+                <c:pt idx="1068">
+                  <c:v>13650</c:v>
+                </c:pt>
+                <c:pt idx="1069">
+                  <c:v>13662</c:v>
+                </c:pt>
+                <c:pt idx="1070">
+                  <c:v>13675</c:v>
+                </c:pt>
+                <c:pt idx="1071">
+                  <c:v>13688</c:v>
+                </c:pt>
+                <c:pt idx="1072">
+                  <c:v>13701</c:v>
+                </c:pt>
+                <c:pt idx="1073">
+                  <c:v>13714</c:v>
+                </c:pt>
+                <c:pt idx="1074">
+                  <c:v>13726</c:v>
+                </c:pt>
+                <c:pt idx="1075">
+                  <c:v>13739</c:v>
+                </c:pt>
+                <c:pt idx="1076">
+                  <c:v>13752</c:v>
+                </c:pt>
+                <c:pt idx="1077">
+                  <c:v>13765</c:v>
+                </c:pt>
+                <c:pt idx="1078">
+                  <c:v>13778</c:v>
+                </c:pt>
+                <c:pt idx="1079">
+                  <c:v>13790</c:v>
+                </c:pt>
+                <c:pt idx="1080">
+                  <c:v>13803</c:v>
+                </c:pt>
+                <c:pt idx="1081">
+                  <c:v>13816</c:v>
+                </c:pt>
+                <c:pt idx="1082">
+                  <c:v>13829</c:v>
+                </c:pt>
+                <c:pt idx="1083">
+                  <c:v>13842</c:v>
+                </c:pt>
+                <c:pt idx="1084">
+                  <c:v>13854</c:v>
+                </c:pt>
+                <c:pt idx="1085">
+                  <c:v>13867</c:v>
+                </c:pt>
+                <c:pt idx="1086">
+                  <c:v>13880</c:v>
+                </c:pt>
+                <c:pt idx="1087">
+                  <c:v>13893</c:v>
+                </c:pt>
+                <c:pt idx="1088">
+                  <c:v>13906</c:v>
+                </c:pt>
+                <c:pt idx="1089">
+                  <c:v>13918</c:v>
+                </c:pt>
+                <c:pt idx="1090">
+                  <c:v>13931</c:v>
+                </c:pt>
+                <c:pt idx="1091">
+                  <c:v>13944</c:v>
+                </c:pt>
+                <c:pt idx="1092">
+                  <c:v>13957</c:v>
+                </c:pt>
+                <c:pt idx="1093">
+                  <c:v>13970</c:v>
+                </c:pt>
+                <c:pt idx="1094">
+                  <c:v>13982</c:v>
+                </c:pt>
+                <c:pt idx="1095">
+                  <c:v>13995</c:v>
+                </c:pt>
+                <c:pt idx="1096">
+                  <c:v>14008</c:v>
+                </c:pt>
+                <c:pt idx="1097">
+                  <c:v>14021</c:v>
+                </c:pt>
+                <c:pt idx="1098">
+                  <c:v>14034</c:v>
+                </c:pt>
+                <c:pt idx="1099">
+                  <c:v>14046</c:v>
+                </c:pt>
+                <c:pt idx="1100">
+                  <c:v>14059</c:v>
+                </c:pt>
+                <c:pt idx="1101">
+                  <c:v>14072</c:v>
+                </c:pt>
+                <c:pt idx="1102">
+                  <c:v>14085</c:v>
+                </c:pt>
+                <c:pt idx="1103">
+                  <c:v>14098</c:v>
+                </c:pt>
+                <c:pt idx="1104">
+                  <c:v>14110</c:v>
+                </c:pt>
+                <c:pt idx="1105">
+                  <c:v>14123</c:v>
+                </c:pt>
+                <c:pt idx="1106">
+                  <c:v>14136</c:v>
+                </c:pt>
+                <c:pt idx="1107">
+                  <c:v>14149</c:v>
+                </c:pt>
+                <c:pt idx="1108">
+                  <c:v>14162</c:v>
+                </c:pt>
+                <c:pt idx="1109">
+                  <c:v>14174</c:v>
+                </c:pt>
+                <c:pt idx="1110">
+                  <c:v>14187</c:v>
+                </c:pt>
+                <c:pt idx="1111">
+                  <c:v>14200</c:v>
+                </c:pt>
+                <c:pt idx="1112">
+                  <c:v>14213</c:v>
+                </c:pt>
+                <c:pt idx="1113">
+                  <c:v>14226</c:v>
+                </c:pt>
+                <c:pt idx="1114">
+                  <c:v>14238</c:v>
+                </c:pt>
+                <c:pt idx="1115">
+                  <c:v>14251</c:v>
+                </c:pt>
+                <c:pt idx="1116">
+                  <c:v>14264</c:v>
+                </c:pt>
+                <c:pt idx="1117">
+                  <c:v>14277</c:v>
+                </c:pt>
+                <c:pt idx="1118">
+                  <c:v>14290</c:v>
+                </c:pt>
+                <c:pt idx="1119">
+                  <c:v>14302</c:v>
+                </c:pt>
+                <c:pt idx="1120">
+                  <c:v>14315</c:v>
+                </c:pt>
+                <c:pt idx="1121">
+                  <c:v>14328</c:v>
+                </c:pt>
+                <c:pt idx="1122">
+                  <c:v>14341</c:v>
+                </c:pt>
+                <c:pt idx="1123">
+                  <c:v>14354</c:v>
+                </c:pt>
+                <c:pt idx="1124">
+                  <c:v>14366</c:v>
+                </c:pt>
+                <c:pt idx="1125">
+                  <c:v>14379</c:v>
+                </c:pt>
+                <c:pt idx="1126">
+                  <c:v>14392</c:v>
+                </c:pt>
+                <c:pt idx="1127">
+                  <c:v>14405</c:v>
+                </c:pt>
+                <c:pt idx="1128">
+                  <c:v>14418</c:v>
+                </c:pt>
+                <c:pt idx="1129">
+                  <c:v>14430</c:v>
+                </c:pt>
+                <c:pt idx="1130">
+                  <c:v>14443</c:v>
+                </c:pt>
+                <c:pt idx="1131">
+                  <c:v>14456</c:v>
+                </c:pt>
+                <c:pt idx="1132">
+                  <c:v>14469</c:v>
+                </c:pt>
+                <c:pt idx="1133">
+                  <c:v>14482</c:v>
+                </c:pt>
+                <c:pt idx="1134">
+                  <c:v>14494</c:v>
+                </c:pt>
+                <c:pt idx="1135">
+                  <c:v>14507</c:v>
+                </c:pt>
+                <c:pt idx="1136">
+                  <c:v>14520</c:v>
+                </c:pt>
+                <c:pt idx="1137">
+                  <c:v>14533</c:v>
+                </c:pt>
+                <c:pt idx="1138">
+                  <c:v>14546</c:v>
+                </c:pt>
+                <c:pt idx="1139">
+                  <c:v>14558</c:v>
+                </c:pt>
+                <c:pt idx="1140">
+                  <c:v>14571</c:v>
+                </c:pt>
+                <c:pt idx="1141">
+                  <c:v>14584</c:v>
+                </c:pt>
+                <c:pt idx="1142">
+                  <c:v>14597</c:v>
+                </c:pt>
+                <c:pt idx="1143">
+                  <c:v>14610</c:v>
+                </c:pt>
+                <c:pt idx="1144">
+                  <c:v>14622</c:v>
+                </c:pt>
+                <c:pt idx="1145">
+                  <c:v>14635</c:v>
+                </c:pt>
+                <c:pt idx="1146">
+                  <c:v>14648</c:v>
+                </c:pt>
+                <c:pt idx="1147">
+                  <c:v>14661</c:v>
+                </c:pt>
+                <c:pt idx="1148">
+                  <c:v>14674</c:v>
+                </c:pt>
+                <c:pt idx="1149">
+                  <c:v>14686</c:v>
+                </c:pt>
+                <c:pt idx="1150">
+                  <c:v>14699</c:v>
+                </c:pt>
+                <c:pt idx="1151">
+                  <c:v>14712</c:v>
+                </c:pt>
+                <c:pt idx="1152">
+                  <c:v>14725</c:v>
+                </c:pt>
+                <c:pt idx="1153">
+                  <c:v>14738</c:v>
+                </c:pt>
+                <c:pt idx="1154">
+                  <c:v>14750</c:v>
+                </c:pt>
+                <c:pt idx="1155">
+                  <c:v>14763</c:v>
+                </c:pt>
+                <c:pt idx="1156">
+                  <c:v>14776</c:v>
+                </c:pt>
+                <c:pt idx="1157">
+                  <c:v>14789</c:v>
+                </c:pt>
+                <c:pt idx="1158">
+                  <c:v>14802</c:v>
+                </c:pt>
+                <c:pt idx="1159">
+                  <c:v>14814</c:v>
+                </c:pt>
+                <c:pt idx="1160">
+                  <c:v>14827</c:v>
+                </c:pt>
+                <c:pt idx="1161">
+                  <c:v>14840</c:v>
+                </c:pt>
+                <c:pt idx="1162">
+                  <c:v>14853</c:v>
+                </c:pt>
+                <c:pt idx="1163">
+                  <c:v>14866</c:v>
+                </c:pt>
+                <c:pt idx="1164">
+                  <c:v>14878</c:v>
+                </c:pt>
+                <c:pt idx="1165">
+                  <c:v>14891</c:v>
+                </c:pt>
+                <c:pt idx="1166">
+                  <c:v>14904</c:v>
+                </c:pt>
+                <c:pt idx="1167">
+                  <c:v>14917</c:v>
+                </c:pt>
+                <c:pt idx="1168">
+                  <c:v>14930</c:v>
+                </c:pt>
+                <c:pt idx="1169">
+                  <c:v>14942</c:v>
+                </c:pt>
+                <c:pt idx="1170">
+                  <c:v>14955</c:v>
+                </c:pt>
+                <c:pt idx="1171">
+                  <c:v>14968</c:v>
+                </c:pt>
+                <c:pt idx="1172">
+                  <c:v>14981</c:v>
+                </c:pt>
+                <c:pt idx="1173">
+                  <c:v>14994</c:v>
+                </c:pt>
+                <c:pt idx="1174">
+                  <c:v>15006</c:v>
+                </c:pt>
+                <c:pt idx="1175">
+                  <c:v>15019</c:v>
+                </c:pt>
+                <c:pt idx="1176">
+                  <c:v>15032</c:v>
+                </c:pt>
+                <c:pt idx="1177">
+                  <c:v>15045</c:v>
+                </c:pt>
+                <c:pt idx="1178">
+                  <c:v>15058</c:v>
+                </c:pt>
+                <c:pt idx="1179">
+                  <c:v>15070</c:v>
+                </c:pt>
+                <c:pt idx="1180">
+                  <c:v>15083</c:v>
+                </c:pt>
+                <c:pt idx="1181">
+                  <c:v>15096</c:v>
+                </c:pt>
+                <c:pt idx="1182">
+                  <c:v>15109</c:v>
+                </c:pt>
+                <c:pt idx="1183">
+                  <c:v>15122</c:v>
+                </c:pt>
+                <c:pt idx="1184">
+                  <c:v>15134</c:v>
+                </c:pt>
+                <c:pt idx="1185">
+                  <c:v>15147</c:v>
+                </c:pt>
+                <c:pt idx="1186">
+                  <c:v>15160</c:v>
+                </c:pt>
+                <c:pt idx="1187">
+                  <c:v>15173</c:v>
+                </c:pt>
+                <c:pt idx="1188">
+                  <c:v>15186</c:v>
+                </c:pt>
+                <c:pt idx="1189">
+                  <c:v>15198</c:v>
+                </c:pt>
+                <c:pt idx="1190">
+                  <c:v>15211</c:v>
+                </c:pt>
+                <c:pt idx="1191">
+                  <c:v>15224</c:v>
+                </c:pt>
+                <c:pt idx="1192">
+                  <c:v>15237</c:v>
+                </c:pt>
+                <c:pt idx="1193">
+                  <c:v>15250</c:v>
+                </c:pt>
+                <c:pt idx="1194">
+                  <c:v>15262</c:v>
+                </c:pt>
+                <c:pt idx="1195">
+                  <c:v>15275</c:v>
+                </c:pt>
+                <c:pt idx="1196">
+                  <c:v>15288</c:v>
+                </c:pt>
+                <c:pt idx="1197">
+                  <c:v>15301</c:v>
+                </c:pt>
+                <c:pt idx="1198">
+                  <c:v>15314</c:v>
+                </c:pt>
+                <c:pt idx="1199">
+                  <c:v>15326</c:v>
+                </c:pt>
+                <c:pt idx="1200">
+                  <c:v>15339</c:v>
+                </c:pt>
+                <c:pt idx="1201">
+                  <c:v>15352</c:v>
+                </c:pt>
+                <c:pt idx="1202">
+                  <c:v>15365</c:v>
+                </c:pt>
+                <c:pt idx="1203">
+                  <c:v>15378</c:v>
+                </c:pt>
+                <c:pt idx="1204">
+                  <c:v>15390</c:v>
+                </c:pt>
+                <c:pt idx="1205">
+                  <c:v>15403</c:v>
+                </c:pt>
+                <c:pt idx="1206">
+                  <c:v>15416</c:v>
+                </c:pt>
+                <c:pt idx="1207">
+                  <c:v>15429</c:v>
+                </c:pt>
+                <c:pt idx="1208">
+                  <c:v>15442</c:v>
+                </c:pt>
+                <c:pt idx="1209">
+                  <c:v>15454</c:v>
+                </c:pt>
+                <c:pt idx="1210">
+                  <c:v>15467</c:v>
+                </c:pt>
+                <c:pt idx="1211">
+                  <c:v>15480</c:v>
+                </c:pt>
+                <c:pt idx="1212">
+                  <c:v>15493</c:v>
+                </c:pt>
+                <c:pt idx="1213">
+                  <c:v>15506</c:v>
+                </c:pt>
+                <c:pt idx="1214">
+                  <c:v>15518</c:v>
+                </c:pt>
+                <c:pt idx="1215">
+                  <c:v>15531</c:v>
+                </c:pt>
+                <c:pt idx="1216">
+                  <c:v>15544</c:v>
+                </c:pt>
+                <c:pt idx="1217">
+                  <c:v>15557</c:v>
+                </c:pt>
+                <c:pt idx="1218">
+                  <c:v>15570</c:v>
+                </c:pt>
+                <c:pt idx="1219">
+                  <c:v>15582</c:v>
+                </c:pt>
+                <c:pt idx="1220">
+                  <c:v>15595</c:v>
+                </c:pt>
+                <c:pt idx="1221">
+                  <c:v>15608</c:v>
+                </c:pt>
+                <c:pt idx="1222">
+                  <c:v>15621</c:v>
+                </c:pt>
+                <c:pt idx="1223">
+                  <c:v>15634</c:v>
+                </c:pt>
+                <c:pt idx="1224">
+                  <c:v>15646</c:v>
+                </c:pt>
+                <c:pt idx="1225">
+                  <c:v>15659</c:v>
+                </c:pt>
+                <c:pt idx="1226">
+                  <c:v>15672</c:v>
+                </c:pt>
+                <c:pt idx="1227">
+                  <c:v>15685</c:v>
+                </c:pt>
+                <c:pt idx="1228">
+                  <c:v>15698</c:v>
+                </c:pt>
+                <c:pt idx="1229">
+                  <c:v>15710</c:v>
+                </c:pt>
+                <c:pt idx="1230">
+                  <c:v>15723</c:v>
+                </c:pt>
+                <c:pt idx="1231">
+                  <c:v>15736</c:v>
+                </c:pt>
+                <c:pt idx="1232">
+                  <c:v>15749</c:v>
+                </c:pt>
+                <c:pt idx="1233">
+                  <c:v>15762</c:v>
+                </c:pt>
+                <c:pt idx="1234">
+                  <c:v>15774</c:v>
+                </c:pt>
+                <c:pt idx="1235">
+                  <c:v>15787</c:v>
+                </c:pt>
+                <c:pt idx="1236">
+                  <c:v>15800</c:v>
+                </c:pt>
+                <c:pt idx="1237">
+                  <c:v>15813</c:v>
+                </c:pt>
+                <c:pt idx="1238">
+                  <c:v>15826</c:v>
+                </c:pt>
+                <c:pt idx="1239">
+                  <c:v>15838</c:v>
+                </c:pt>
+                <c:pt idx="1240">
+                  <c:v>15851</c:v>
+                </c:pt>
+                <c:pt idx="1241">
+                  <c:v>15864</c:v>
+                </c:pt>
+                <c:pt idx="1242">
+                  <c:v>15877</c:v>
+                </c:pt>
+                <c:pt idx="1243">
+                  <c:v>15890</c:v>
+                </c:pt>
+                <c:pt idx="1244">
+                  <c:v>15902</c:v>
+                </c:pt>
+                <c:pt idx="1245">
+                  <c:v>15915</c:v>
+                </c:pt>
+                <c:pt idx="1246">
+                  <c:v>15928</c:v>
+                </c:pt>
+                <c:pt idx="1247">
+                  <c:v>15941</c:v>
+                </c:pt>
+                <c:pt idx="1248">
+                  <c:v>15954</c:v>
+                </c:pt>
+                <c:pt idx="1249">
+                  <c:v>15966</c:v>
+                </c:pt>
+                <c:pt idx="1250">
+                  <c:v>15979</c:v>
+                </c:pt>
+                <c:pt idx="1251">
+                  <c:v>15992</c:v>
+                </c:pt>
+                <c:pt idx="1252">
+                  <c:v>16005</c:v>
+                </c:pt>
+                <c:pt idx="1253">
+                  <c:v>16018</c:v>
+                </c:pt>
+                <c:pt idx="1254">
+                  <c:v>16030</c:v>
+                </c:pt>
+                <c:pt idx="1255">
+                  <c:v>16043</c:v>
+                </c:pt>
+                <c:pt idx="1256">
+                  <c:v>16056</c:v>
+                </c:pt>
+                <c:pt idx="1257">
+                  <c:v>16069</c:v>
+                </c:pt>
+                <c:pt idx="1258">
+                  <c:v>16082</c:v>
+                </c:pt>
+                <c:pt idx="1259">
+                  <c:v>16094</c:v>
+                </c:pt>
+                <c:pt idx="1260">
+                  <c:v>16107</c:v>
+                </c:pt>
+                <c:pt idx="1261">
+                  <c:v>16120</c:v>
+                </c:pt>
+                <c:pt idx="1262">
+                  <c:v>16133</c:v>
+                </c:pt>
+                <c:pt idx="1263">
+                  <c:v>16146</c:v>
+                </c:pt>
+                <c:pt idx="1264">
+                  <c:v>16158</c:v>
+                </c:pt>
+                <c:pt idx="1265">
+                  <c:v>16171</c:v>
+                </c:pt>
+                <c:pt idx="1266">
+                  <c:v>16184</c:v>
+                </c:pt>
+                <c:pt idx="1267">
+                  <c:v>16197</c:v>
+                </c:pt>
+                <c:pt idx="1268">
+                  <c:v>16210</c:v>
+                </c:pt>
+                <c:pt idx="1269">
+                  <c:v>16222</c:v>
+                </c:pt>
+                <c:pt idx="1270">
+                  <c:v>16235</c:v>
+                </c:pt>
+                <c:pt idx="1271">
+                  <c:v>16248</c:v>
+                </c:pt>
+                <c:pt idx="1272">
+                  <c:v>16261</c:v>
+                </c:pt>
+                <c:pt idx="1273">
+                  <c:v>16274</c:v>
+                </c:pt>
+                <c:pt idx="1274">
+                  <c:v>16286</c:v>
+                </c:pt>
+                <c:pt idx="1275">
+                  <c:v>16299</c:v>
+                </c:pt>
+                <c:pt idx="1276">
+                  <c:v>16312</c:v>
+                </c:pt>
+                <c:pt idx="1277">
+                  <c:v>16325</c:v>
+                </c:pt>
+                <c:pt idx="1278">
+                  <c:v>16338</c:v>
+                </c:pt>
+                <c:pt idx="1279">
+                  <c:v>16350</c:v>
+                </c:pt>
+                <c:pt idx="1280">
+                  <c:v>16363</c:v>
+                </c:pt>
+                <c:pt idx="1281">
+                  <c:v>16376</c:v>
+                </c:pt>
+                <c:pt idx="1282">
+                  <c:v>16389</c:v>
+                </c:pt>
+                <c:pt idx="1283">
+                  <c:v>16402</c:v>
+                </c:pt>
+                <c:pt idx="1284">
+                  <c:v>16414</c:v>
+                </c:pt>
+                <c:pt idx="1285">
+                  <c:v>16427</c:v>
+                </c:pt>
+                <c:pt idx="1286">
+                  <c:v>16440</c:v>
+                </c:pt>
+                <c:pt idx="1287">
+                  <c:v>16453</c:v>
+                </c:pt>
+                <c:pt idx="1288">
+                  <c:v>16466</c:v>
+                </c:pt>
+                <c:pt idx="1289">
+                  <c:v>16478</c:v>
+                </c:pt>
+                <c:pt idx="1290">
+                  <c:v>16491</c:v>
+                </c:pt>
+                <c:pt idx="1291">
+                  <c:v>16504</c:v>
+                </c:pt>
+                <c:pt idx="1292">
+                  <c:v>16517</c:v>
+                </c:pt>
+                <c:pt idx="1293">
+                  <c:v>16530</c:v>
+                </c:pt>
+                <c:pt idx="1294">
+                  <c:v>16542</c:v>
+                </c:pt>
+                <c:pt idx="1295">
+                  <c:v>16555</c:v>
+                </c:pt>
+                <c:pt idx="1296">
+                  <c:v>16568</c:v>
+                </c:pt>
+                <c:pt idx="1297">
+                  <c:v>16581</c:v>
+                </c:pt>
+                <c:pt idx="1298">
+                  <c:v>16594</c:v>
+                </c:pt>
+                <c:pt idx="1299">
+                  <c:v>16606</c:v>
+                </c:pt>
+                <c:pt idx="1300">
+                  <c:v>16619</c:v>
+                </c:pt>
+                <c:pt idx="1301">
+                  <c:v>16632</c:v>
+                </c:pt>
+                <c:pt idx="1302">
+                  <c:v>16645</c:v>
+                </c:pt>
+                <c:pt idx="1303">
+                  <c:v>16658</c:v>
+                </c:pt>
+                <c:pt idx="1304">
+                  <c:v>16670</c:v>
+                </c:pt>
+                <c:pt idx="1305">
+                  <c:v>16683</c:v>
+                </c:pt>
+                <c:pt idx="1306">
+                  <c:v>16696</c:v>
+                </c:pt>
+                <c:pt idx="1307">
+                  <c:v>16709</c:v>
+                </c:pt>
+                <c:pt idx="1308">
+                  <c:v>16722</c:v>
+                </c:pt>
+                <c:pt idx="1309">
+                  <c:v>16734</c:v>
+                </c:pt>
+                <c:pt idx="1310">
+                  <c:v>16747</c:v>
+                </c:pt>
+                <c:pt idx="1311">
+                  <c:v>16760</c:v>
+                </c:pt>
+                <c:pt idx="1312">
+                  <c:v>16773</c:v>
+                </c:pt>
+                <c:pt idx="1313">
+                  <c:v>16786</c:v>
+                </c:pt>
+                <c:pt idx="1314">
+                  <c:v>16798</c:v>
+                </c:pt>
+                <c:pt idx="1315">
+                  <c:v>16811</c:v>
+                </c:pt>
+                <c:pt idx="1316">
+                  <c:v>16824</c:v>
+                </c:pt>
+                <c:pt idx="1317">
+                  <c:v>16837</c:v>
+                </c:pt>
+                <c:pt idx="1318">
+                  <c:v>16850</c:v>
+                </c:pt>
+                <c:pt idx="1319">
+                  <c:v>16862</c:v>
+                </c:pt>
+                <c:pt idx="1320">
+                  <c:v>16875</c:v>
+                </c:pt>
+                <c:pt idx="1321">
+                  <c:v>16888</c:v>
+                </c:pt>
+                <c:pt idx="1322">
+                  <c:v>16901</c:v>
+                </c:pt>
+                <c:pt idx="1323">
+                  <c:v>16914</c:v>
+                </c:pt>
+                <c:pt idx="1324">
+                  <c:v>16926</c:v>
+                </c:pt>
+                <c:pt idx="1325">
+                  <c:v>16939</c:v>
+                </c:pt>
+                <c:pt idx="1326">
+                  <c:v>16952</c:v>
+                </c:pt>
+                <c:pt idx="1327">
+                  <c:v>16965</c:v>
+                </c:pt>
+                <c:pt idx="1328">
+                  <c:v>16978</c:v>
+                </c:pt>
+                <c:pt idx="1329">
+                  <c:v>16990</c:v>
+                </c:pt>
+                <c:pt idx="1330">
+                  <c:v>17003</c:v>
+                </c:pt>
+                <c:pt idx="1331">
+                  <c:v>17016</c:v>
+                </c:pt>
+                <c:pt idx="1332">
+                  <c:v>17029</c:v>
+                </c:pt>
+                <c:pt idx="1333">
+                  <c:v>17042</c:v>
+                </c:pt>
+                <c:pt idx="1334">
+                  <c:v>17054</c:v>
+                </c:pt>
+                <c:pt idx="1335">
+                  <c:v>17067</c:v>
+                </c:pt>
+                <c:pt idx="1336">
+                  <c:v>17080</c:v>
+                </c:pt>
+                <c:pt idx="1337">
+                  <c:v>17093</c:v>
+                </c:pt>
+                <c:pt idx="1338">
+                  <c:v>17106</c:v>
+                </c:pt>
+                <c:pt idx="1339">
+                  <c:v>17118</c:v>
+                </c:pt>
+                <c:pt idx="1340">
+                  <c:v>17131</c:v>
+                </c:pt>
+                <c:pt idx="1341">
+                  <c:v>17144</c:v>
+                </c:pt>
+                <c:pt idx="1342">
+                  <c:v>17157</c:v>
+                </c:pt>
+                <c:pt idx="1343">
+                  <c:v>17170</c:v>
+                </c:pt>
+                <c:pt idx="1344">
+                  <c:v>17182</c:v>
+                </c:pt>
+                <c:pt idx="1345">
+                  <c:v>17195</c:v>
+                </c:pt>
+                <c:pt idx="1346">
+                  <c:v>17208</c:v>
+                </c:pt>
+                <c:pt idx="1347">
+                  <c:v>17221</c:v>
+                </c:pt>
+                <c:pt idx="1348">
+                  <c:v>17234</c:v>
+                </c:pt>
+                <c:pt idx="1349">
+                  <c:v>17246</c:v>
+                </c:pt>
+                <c:pt idx="1350">
+                  <c:v>17259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>keep.7ep2!$J:$J</c:f>
+              <c:f>keep.7ep4!$J:$J</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1048576"/>
@@ -10766,6 +11777,1017 @@
                 </c:pt>
                 <c:pt idx="1013">
                   <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1014">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1015">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1016">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1017">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1018">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1019">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1020">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1021">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1022">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1023">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1024">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1025">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1026">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1027">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1028">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1029">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1030">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1031">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1032">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1033">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1034">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1035">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1036">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1037">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1038">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1039">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1040">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1041">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1042">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1043">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1044">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1045">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1046">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1047">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1048">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1049">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1050">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1051">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1052">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1053">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1054">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1055">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1056">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1057">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1058">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1059">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1060">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1061">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1062">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1063">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1064">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1065">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1066">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1067">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1068">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1069">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1070">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1071">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1072">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1073">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1074">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1075">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1076">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1077">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1078">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1079">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1080">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1081">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1082">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1083">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1084">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1085">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1086">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1087">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1088">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1089">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1090">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1091">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1092">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1093">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1094">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1095">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1096">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1097">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1098">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1099">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1100">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1101">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1102">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1103">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1104">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1105">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1106">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1107">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1108">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1109">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1110">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1111">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1112">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1113">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1114">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1115">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1116">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1117">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1118">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1119">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1120">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1121">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1122">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1123">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1124">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1125">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1126">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1127">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1128">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1129">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1130">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1131">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1132">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1133">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1134">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1135">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1136">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1137">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1138">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1139">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1140">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1141">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1142">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1143">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1144">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1145">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1146">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1147">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1148">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1149">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1150">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1151">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1152">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1153">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1154">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1155">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1156">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1157">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1158">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1159">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1160">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1161">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1162">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1163">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1164">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1165">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1166">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1167">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1168">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1169">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1170">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1171">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1172">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1173">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1174">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1175">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1176">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1177">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1178">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1179">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1180">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1181">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1182">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1183">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1184">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1185">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1186">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1187">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1188">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1189">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1190">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1191">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1192">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1193">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1194">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1195">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1196">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1197">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1198">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1199">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1200">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1201">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1202">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1203">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1204">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1205">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1206">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1207">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1208">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1209">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1210">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1211">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1212">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1213">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1214">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1215">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1216">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1217">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1218">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1219">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1220">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1221">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1222">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1223">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1224">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1225">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1226">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1227">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1228">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1229">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1230">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1231">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1232">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1233">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1234">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1235">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1236">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1237">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1238">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1239">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1240">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1241">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1242">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1243">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1244">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1245">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1246">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1247">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1248">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1249">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1250">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1251">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1252">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1253">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1254">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1255">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1256">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1257">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1258">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1259">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1260">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1261">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1262">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1263">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1264">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1265">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1266">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1267">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1268">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1269">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1270">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1271">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1272">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1273">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1274">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1275">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1276">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1277">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1278">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1279">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1280">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1281">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1282">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1283">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1284">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1285">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1286">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1287">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1288">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1289">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1290">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1291">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1292">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1293">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1294">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1295">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1296">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1297">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1298">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1299">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1300">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1301">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1302">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1303">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1304">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1305">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1306">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1307">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1308">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1309">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1310">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1311">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1312">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1313">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1314">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1315">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1316">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1317">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1318">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1319">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1320">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1321">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1322">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1323">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1324">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1325">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1326">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1327">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1328">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1329">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1330">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1331">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1332">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1333">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1334">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1335">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1336">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1337">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1338">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1339">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1340">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1341">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1342">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1343">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1344">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1345">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1346">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1347">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1348">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1349">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1350">
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12885,7 +14907,7 @@
         <c:axId val="1341699184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="13000"/>
+          <c:max val="17500"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -15412,6 +17434,162 @@
       </cdr:style>
     </cdr:cxnSp>
   </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.7673</cdr:x>
+      <cdr:y>0.66656</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91081</cdr:x>
+      <cdr:y>0.76154</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A269AA-C5B9-4EA6-B149-29D00422E0C3}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6638725" y="4179104"/>
+          <a:ext cx="1241706" cy="595453"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Realoaded training data</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73608</cdr:x>
+      <cdr:y>0.74964</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.77509</cdr:x>
+      <cdr:y>0.87426</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69047DA2-F071-4CB1-9456-9AB2B6126280}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="6368648" y="4699965"/>
+          <a:ext cx="337518" cy="781320"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
 
@@ -46356,10 +48534,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815C02E8-8348-4DD9-A251-1AE6A6F46CEC}">
-  <dimension ref="A1:J1014"/>
+  <dimension ref="A1:J1351"/>
   <sheetViews>
-    <sheetView topLeftCell="A659" workbookViewId="0">
-      <selection activeCell="I674" sqref="I674"/>
+    <sheetView topLeftCell="A1336" workbookViewId="0">
+      <selection activeCell="N1344" sqref="N1344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -76709,6 +78887,2702 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
+    <row r="1015" spans="1:10">
+      <c r="F1015">
+        <v>12958</v>
+      </c>
+      <c r="J1015">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:10">
+      <c r="F1016">
+        <v>12971</v>
+      </c>
+      <c r="J1016">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:10">
+      <c r="F1017">
+        <v>12984</v>
+      </c>
+      <c r="J1017">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:10">
+      <c r="F1018">
+        <v>12997</v>
+      </c>
+      <c r="J1018">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:10">
+      <c r="F1019">
+        <v>13010</v>
+      </c>
+      <c r="J1019">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:10">
+      <c r="F1020">
+        <v>13022</v>
+      </c>
+      <c r="J1020">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:10">
+      <c r="F1021">
+        <v>13035</v>
+      </c>
+      <c r="J1021">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:10">
+      <c r="F1022">
+        <v>13048</v>
+      </c>
+      <c r="J1022">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:10">
+      <c r="F1023">
+        <v>13061</v>
+      </c>
+      <c r="J1023">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:10">
+      <c r="F1024">
+        <v>13074</v>
+      </c>
+      <c r="J1024">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1025" spans="6:10">
+      <c r="F1025">
+        <v>13086</v>
+      </c>
+      <c r="J1025">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1026" spans="6:10">
+      <c r="F1026">
+        <v>13099</v>
+      </c>
+      <c r="J1026">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1027" spans="6:10">
+      <c r="F1027">
+        <v>13112</v>
+      </c>
+      <c r="J1027">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1028" spans="6:10">
+      <c r="F1028">
+        <v>13125</v>
+      </c>
+      <c r="J1028">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1029" spans="6:10">
+      <c r="F1029">
+        <v>13138</v>
+      </c>
+      <c r="J1029">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1030" spans="6:10">
+      <c r="F1030">
+        <v>13150</v>
+      </c>
+      <c r="J1030">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1031" spans="6:10">
+      <c r="F1031">
+        <v>13163</v>
+      </c>
+      <c r="J1031">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1032" spans="6:10">
+      <c r="F1032">
+        <v>13176</v>
+      </c>
+      <c r="J1032">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1033" spans="6:10">
+      <c r="F1033">
+        <v>13189</v>
+      </c>
+      <c r="J1033">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1034" spans="6:10">
+      <c r="F1034">
+        <v>13202</v>
+      </c>
+      <c r="J1034">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1035" spans="6:10">
+      <c r="F1035">
+        <v>13214</v>
+      </c>
+      <c r="J1035">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1036" spans="6:10">
+      <c r="F1036">
+        <v>13227</v>
+      </c>
+      <c r="J1036">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1037" spans="6:10">
+      <c r="F1037">
+        <v>13240</v>
+      </c>
+      <c r="J1037">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1038" spans="6:10">
+      <c r="F1038">
+        <v>13253</v>
+      </c>
+      <c r="J1038">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1039" spans="6:10">
+      <c r="F1039">
+        <v>13266</v>
+      </c>
+      <c r="J1039">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1040" spans="6:10">
+      <c r="F1040">
+        <v>13278</v>
+      </c>
+      <c r="J1040">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1041" spans="6:10">
+      <c r="F1041">
+        <v>13291</v>
+      </c>
+      <c r="J1041">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1042" spans="6:10">
+      <c r="F1042">
+        <v>13304</v>
+      </c>
+      <c r="J1042">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1043" spans="6:10">
+      <c r="F1043">
+        <v>13317</v>
+      </c>
+      <c r="J1043">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1044" spans="6:10">
+      <c r="F1044">
+        <v>13330</v>
+      </c>
+      <c r="J1044">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1045" spans="6:10">
+      <c r="F1045">
+        <v>13342</v>
+      </c>
+      <c r="J1045">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1046" spans="6:10">
+      <c r="F1046">
+        <v>13355</v>
+      </c>
+      <c r="J1046">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1047" spans="6:10">
+      <c r="F1047">
+        <v>13368</v>
+      </c>
+      <c r="J1047">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1048" spans="6:10">
+      <c r="F1048">
+        <v>13381</v>
+      </c>
+      <c r="J1048">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1049" spans="6:10">
+      <c r="F1049">
+        <v>13394</v>
+      </c>
+      <c r="J1049">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1050" spans="6:10">
+      <c r="F1050">
+        <v>13406</v>
+      </c>
+      <c r="J1050">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1051" spans="6:10">
+      <c r="F1051">
+        <v>13419</v>
+      </c>
+      <c r="J1051">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1052" spans="6:10">
+      <c r="F1052">
+        <v>13432</v>
+      </c>
+      <c r="J1052">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1053" spans="6:10">
+      <c r="F1053">
+        <v>13445</v>
+      </c>
+      <c r="J1053">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1054" spans="6:10">
+      <c r="F1054">
+        <v>13458</v>
+      </c>
+      <c r="J1054">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1055" spans="6:10">
+      <c r="F1055">
+        <v>13470</v>
+      </c>
+      <c r="J1055">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1056" spans="6:10">
+      <c r="F1056">
+        <v>13483</v>
+      </c>
+      <c r="J1056">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1057" spans="6:10">
+      <c r="F1057">
+        <v>13496</v>
+      </c>
+      <c r="J1057">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1058" spans="6:10">
+      <c r="F1058">
+        <v>13509</v>
+      </c>
+      <c r="J1058">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1059" spans="6:10">
+      <c r="F1059">
+        <v>13522</v>
+      </c>
+      <c r="J1059">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1060" spans="6:10">
+      <c r="F1060">
+        <v>13534</v>
+      </c>
+      <c r="J1060">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1061" spans="6:10">
+      <c r="F1061">
+        <v>13547</v>
+      </c>
+      <c r="J1061">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1062" spans="6:10">
+      <c r="F1062">
+        <v>13560</v>
+      </c>
+      <c r="J1062">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1063" spans="6:10">
+      <c r="F1063">
+        <v>13573</v>
+      </c>
+      <c r="J1063">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1064" spans="6:10">
+      <c r="F1064">
+        <v>13586</v>
+      </c>
+      <c r="J1064">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1065" spans="6:10">
+      <c r="F1065">
+        <v>13598</v>
+      </c>
+      <c r="J1065">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1066" spans="6:10">
+      <c r="F1066">
+        <v>13611</v>
+      </c>
+      <c r="J1066">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1067" spans="6:10">
+      <c r="F1067">
+        <v>13624</v>
+      </c>
+      <c r="J1067">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1068" spans="6:10">
+      <c r="F1068">
+        <v>13637</v>
+      </c>
+      <c r="J1068">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1069" spans="6:10">
+      <c r="F1069">
+        <v>13650</v>
+      </c>
+      <c r="J1069">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1070" spans="6:10">
+      <c r="F1070">
+        <v>13662</v>
+      </c>
+      <c r="J1070">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1071" spans="6:10">
+      <c r="F1071">
+        <v>13675</v>
+      </c>
+      <c r="J1071">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1072" spans="6:10">
+      <c r="F1072">
+        <v>13688</v>
+      </c>
+      <c r="J1072">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1073" spans="6:10">
+      <c r="F1073">
+        <v>13701</v>
+      </c>
+      <c r="J1073">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1074" spans="6:10">
+      <c r="F1074">
+        <v>13714</v>
+      </c>
+      <c r="J1074">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1075" spans="6:10">
+      <c r="F1075">
+        <v>13726</v>
+      </c>
+      <c r="J1075">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1076" spans="6:10">
+      <c r="F1076">
+        <v>13739</v>
+      </c>
+      <c r="J1076">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1077" spans="6:10">
+      <c r="F1077">
+        <v>13752</v>
+      </c>
+      <c r="J1077">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1078" spans="6:10">
+      <c r="F1078">
+        <v>13765</v>
+      </c>
+      <c r="J1078">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1079" spans="6:10">
+      <c r="F1079">
+        <v>13778</v>
+      </c>
+      <c r="J1079">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1080" spans="6:10">
+      <c r="F1080">
+        <v>13790</v>
+      </c>
+      <c r="J1080">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1081" spans="6:10">
+      <c r="F1081">
+        <v>13803</v>
+      </c>
+      <c r="J1081">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1082" spans="6:10">
+      <c r="F1082">
+        <v>13816</v>
+      </c>
+      <c r="J1082">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1083" spans="6:10">
+      <c r="F1083">
+        <v>13829</v>
+      </c>
+      <c r="J1083">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1084" spans="6:10">
+      <c r="F1084">
+        <v>13842</v>
+      </c>
+      <c r="J1084">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1085" spans="6:10">
+      <c r="F1085">
+        <v>13854</v>
+      </c>
+      <c r="J1085">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1086" spans="6:10">
+      <c r="F1086">
+        <v>13867</v>
+      </c>
+      <c r="J1086">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1087" spans="6:10">
+      <c r="F1087">
+        <v>13880</v>
+      </c>
+      <c r="J1087">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1088" spans="6:10">
+      <c r="F1088">
+        <v>13893</v>
+      </c>
+      <c r="J1088">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1089" spans="6:10">
+      <c r="F1089">
+        <v>13906</v>
+      </c>
+      <c r="J1089">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1090" spans="6:10">
+      <c r="F1090">
+        <v>13918</v>
+      </c>
+      <c r="J1090">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1091" spans="6:10">
+      <c r="F1091">
+        <v>13931</v>
+      </c>
+      <c r="J1091">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1092" spans="6:10">
+      <c r="F1092">
+        <v>13944</v>
+      </c>
+      <c r="J1092">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1093" spans="6:10">
+      <c r="F1093">
+        <v>13957</v>
+      </c>
+      <c r="J1093">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1094" spans="6:10">
+      <c r="F1094">
+        <v>13970</v>
+      </c>
+      <c r="J1094">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1095" spans="6:10">
+      <c r="F1095">
+        <v>13982</v>
+      </c>
+      <c r="J1095">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1096" spans="6:10">
+      <c r="F1096">
+        <v>13995</v>
+      </c>
+      <c r="J1096">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1097" spans="6:10">
+      <c r="F1097">
+        <v>14008</v>
+      </c>
+      <c r="J1097">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1098" spans="6:10">
+      <c r="F1098">
+        <v>14021</v>
+      </c>
+      <c r="J1098">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1099" spans="6:10">
+      <c r="F1099">
+        <v>14034</v>
+      </c>
+      <c r="J1099">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1100" spans="6:10">
+      <c r="F1100">
+        <v>14046</v>
+      </c>
+      <c r="J1100">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1101" spans="6:10">
+      <c r="F1101">
+        <v>14059</v>
+      </c>
+      <c r="J1101">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1102" spans="6:10">
+      <c r="F1102">
+        <v>14072</v>
+      </c>
+      <c r="J1102">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1103" spans="6:10">
+      <c r="F1103">
+        <v>14085</v>
+      </c>
+      <c r="J1103">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1104" spans="6:10">
+      <c r="F1104">
+        <v>14098</v>
+      </c>
+      <c r="J1104">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1105" spans="6:10">
+      <c r="F1105">
+        <v>14110</v>
+      </c>
+      <c r="J1105">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1106" spans="6:10">
+      <c r="F1106">
+        <v>14123</v>
+      </c>
+      <c r="J1106">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1107" spans="6:10">
+      <c r="F1107">
+        <v>14136</v>
+      </c>
+      <c r="J1107">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1108" spans="6:10">
+      <c r="F1108">
+        <v>14149</v>
+      </c>
+      <c r="J1108">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1109" spans="6:10">
+      <c r="F1109">
+        <v>14162</v>
+      </c>
+      <c r="J1109">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1110" spans="6:10">
+      <c r="F1110">
+        <v>14174</v>
+      </c>
+      <c r="J1110">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1111" spans="6:10">
+      <c r="F1111">
+        <v>14187</v>
+      </c>
+      <c r="J1111">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1112" spans="6:10">
+      <c r="F1112">
+        <v>14200</v>
+      </c>
+      <c r="J1112">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1113" spans="6:10">
+      <c r="F1113">
+        <v>14213</v>
+      </c>
+      <c r="J1113">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1114" spans="6:10">
+      <c r="F1114">
+        <v>14226</v>
+      </c>
+      <c r="J1114">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1115" spans="6:10">
+      <c r="F1115">
+        <v>14238</v>
+      </c>
+      <c r="J1115">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1116" spans="6:10">
+      <c r="F1116">
+        <v>14251</v>
+      </c>
+      <c r="J1116">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1117" spans="6:10">
+      <c r="F1117">
+        <v>14264</v>
+      </c>
+      <c r="J1117">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1118" spans="6:10">
+      <c r="F1118">
+        <v>14277</v>
+      </c>
+      <c r="J1118">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1119" spans="6:10">
+      <c r="F1119">
+        <v>14290</v>
+      </c>
+      <c r="J1119">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1120" spans="6:10">
+      <c r="F1120">
+        <v>14302</v>
+      </c>
+      <c r="J1120">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1121" spans="6:10">
+      <c r="F1121">
+        <v>14315</v>
+      </c>
+      <c r="J1121">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1122" spans="6:10">
+      <c r="F1122">
+        <v>14328</v>
+      </c>
+      <c r="J1122">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1123" spans="6:10">
+      <c r="F1123">
+        <v>14341</v>
+      </c>
+      <c r="J1123">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1124" spans="6:10">
+      <c r="F1124">
+        <v>14354</v>
+      </c>
+      <c r="J1124">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1125" spans="6:10">
+      <c r="F1125">
+        <v>14366</v>
+      </c>
+      <c r="J1125">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1126" spans="6:10">
+      <c r="F1126">
+        <v>14379</v>
+      </c>
+      <c r="J1126">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1127" spans="6:10">
+      <c r="F1127">
+        <v>14392</v>
+      </c>
+      <c r="J1127">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1128" spans="6:10">
+      <c r="F1128">
+        <v>14405</v>
+      </c>
+      <c r="J1128">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="1129" spans="6:10">
+      <c r="F1129">
+        <v>14418</v>
+      </c>
+      <c r="J1129">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1130" spans="6:10">
+      <c r="F1130">
+        <v>14430</v>
+      </c>
+      <c r="J1130">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="1131" spans="6:10">
+      <c r="F1131">
+        <v>14443</v>
+      </c>
+      <c r="J1131">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1132" spans="6:10">
+      <c r="F1132">
+        <v>14456</v>
+      </c>
+      <c r="J1132">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1133" spans="6:10">
+      <c r="F1133">
+        <v>14469</v>
+      </c>
+      <c r="J1133">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1134" spans="6:10">
+      <c r="F1134">
+        <v>14482</v>
+      </c>
+      <c r="J1134">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1135" spans="6:10">
+      <c r="F1135">
+        <v>14494</v>
+      </c>
+      <c r="J1135">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1136" spans="6:10">
+      <c r="F1136">
+        <v>14507</v>
+      </c>
+      <c r="J1136">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1137" spans="6:10">
+      <c r="F1137">
+        <v>14520</v>
+      </c>
+      <c r="J1137">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1138" spans="6:10">
+      <c r="F1138">
+        <v>14533</v>
+      </c>
+      <c r="J1138">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1139" spans="6:10">
+      <c r="F1139">
+        <v>14546</v>
+      </c>
+      <c r="J1139">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1140" spans="6:10">
+      <c r="F1140">
+        <v>14558</v>
+      </c>
+      <c r="J1140">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1141" spans="6:10">
+      <c r="F1141">
+        <v>14571</v>
+      </c>
+      <c r="J1141">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1142" spans="6:10">
+      <c r="F1142">
+        <v>14584</v>
+      </c>
+      <c r="J1142">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1143" spans="6:10">
+      <c r="F1143">
+        <v>14597</v>
+      </c>
+      <c r="J1143">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1144" spans="6:10">
+      <c r="F1144">
+        <v>14610</v>
+      </c>
+      <c r="J1144">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1145" spans="6:10">
+      <c r="F1145">
+        <v>14622</v>
+      </c>
+      <c r="J1145">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1146" spans="6:10">
+      <c r="F1146">
+        <v>14635</v>
+      </c>
+      <c r="J1146">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1147" spans="6:10">
+      <c r="F1147">
+        <v>14648</v>
+      </c>
+      <c r="J1147">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1148" spans="6:10">
+      <c r="F1148">
+        <v>14661</v>
+      </c>
+      <c r="J1148">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1149" spans="6:10">
+      <c r="F1149">
+        <v>14674</v>
+      </c>
+      <c r="J1149">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1150" spans="6:10">
+      <c r="F1150">
+        <v>14686</v>
+      </c>
+      <c r="J1150">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1151" spans="6:10">
+      <c r="F1151">
+        <v>14699</v>
+      </c>
+      <c r="J1151">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1152" spans="6:10">
+      <c r="F1152">
+        <v>14712</v>
+      </c>
+      <c r="J1152">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1153" spans="6:10">
+      <c r="F1153">
+        <v>14725</v>
+      </c>
+      <c r="J1153">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1154" spans="6:10">
+      <c r="F1154">
+        <v>14738</v>
+      </c>
+      <c r="J1154">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1155" spans="6:10">
+      <c r="F1155">
+        <v>14750</v>
+      </c>
+      <c r="J1155">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1156" spans="6:10">
+      <c r="F1156">
+        <v>14763</v>
+      </c>
+      <c r="J1156">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1157" spans="6:10">
+      <c r="F1157">
+        <v>14776</v>
+      </c>
+      <c r="J1157">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1158" spans="6:10">
+      <c r="F1158">
+        <v>14789</v>
+      </c>
+      <c r="J1158">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1159" spans="6:10">
+      <c r="F1159">
+        <v>14802</v>
+      </c>
+      <c r="J1159">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1160" spans="6:10">
+      <c r="F1160">
+        <v>14814</v>
+      </c>
+      <c r="J1160">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1161" spans="6:10">
+      <c r="F1161">
+        <v>14827</v>
+      </c>
+      <c r="J1161">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1162" spans="6:10">
+      <c r="F1162">
+        <v>14840</v>
+      </c>
+      <c r="J1162">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1163" spans="6:10">
+      <c r="F1163">
+        <v>14853</v>
+      </c>
+      <c r="J1163">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1164" spans="6:10">
+      <c r="F1164">
+        <v>14866</v>
+      </c>
+      <c r="J1164">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1165" spans="6:10">
+      <c r="F1165">
+        <v>14878</v>
+      </c>
+      <c r="J1165">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1166" spans="6:10">
+      <c r="F1166">
+        <v>14891</v>
+      </c>
+      <c r="J1166">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1167" spans="6:10">
+      <c r="F1167">
+        <v>14904</v>
+      </c>
+      <c r="J1167">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1168" spans="6:10">
+      <c r="F1168">
+        <v>14917</v>
+      </c>
+      <c r="J1168">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1169" spans="6:10">
+      <c r="F1169">
+        <v>14930</v>
+      </c>
+      <c r="J1169">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1170" spans="6:10">
+      <c r="F1170">
+        <v>14942</v>
+      </c>
+      <c r="J1170">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1171" spans="6:10">
+      <c r="F1171">
+        <v>14955</v>
+      </c>
+      <c r="J1171">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1172" spans="6:10">
+      <c r="F1172">
+        <v>14968</v>
+      </c>
+      <c r="J1172">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1173" spans="6:10">
+      <c r="F1173">
+        <v>14981</v>
+      </c>
+      <c r="J1173">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1174" spans="6:10">
+      <c r="F1174">
+        <v>14994</v>
+      </c>
+      <c r="J1174">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1175" spans="6:10">
+      <c r="F1175">
+        <v>15006</v>
+      </c>
+      <c r="J1175">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1176" spans="6:10">
+      <c r="F1176">
+        <v>15019</v>
+      </c>
+      <c r="J1176">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1177" spans="6:10">
+      <c r="F1177">
+        <v>15032</v>
+      </c>
+      <c r="J1177">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1178" spans="6:10">
+      <c r="F1178">
+        <v>15045</v>
+      </c>
+      <c r="J1178">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1179" spans="6:10">
+      <c r="F1179">
+        <v>15058</v>
+      </c>
+      <c r="J1179">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1180" spans="6:10">
+      <c r="F1180">
+        <v>15070</v>
+      </c>
+      <c r="J1180">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1181" spans="6:10">
+      <c r="F1181">
+        <v>15083</v>
+      </c>
+      <c r="J1181">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1182" spans="6:10">
+      <c r="F1182">
+        <v>15096</v>
+      </c>
+      <c r="J1182">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1183" spans="6:10">
+      <c r="F1183">
+        <v>15109</v>
+      </c>
+      <c r="J1183">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1184" spans="6:10">
+      <c r="F1184">
+        <v>15122</v>
+      </c>
+      <c r="J1184">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1185" spans="6:10">
+      <c r="F1185">
+        <v>15134</v>
+      </c>
+      <c r="J1185">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1186" spans="6:10">
+      <c r="F1186">
+        <v>15147</v>
+      </c>
+      <c r="J1186">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1187" spans="6:10">
+      <c r="F1187">
+        <v>15160</v>
+      </c>
+      <c r="J1187">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1188" spans="6:10">
+      <c r="F1188">
+        <v>15173</v>
+      </c>
+      <c r="J1188">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1189" spans="6:10">
+      <c r="F1189">
+        <v>15186</v>
+      </c>
+      <c r="J1189">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1190" spans="6:10">
+      <c r="F1190">
+        <v>15198</v>
+      </c>
+      <c r="J1190">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1191" spans="6:10">
+      <c r="F1191">
+        <v>15211</v>
+      </c>
+      <c r="J1191">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1192" spans="6:10">
+      <c r="F1192">
+        <v>15224</v>
+      </c>
+      <c r="J1192">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1193" spans="6:10">
+      <c r="F1193">
+        <v>15237</v>
+      </c>
+      <c r="J1193">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1194" spans="6:10">
+      <c r="F1194">
+        <v>15250</v>
+      </c>
+      <c r="J1194">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1195" spans="6:10">
+      <c r="F1195">
+        <v>15262</v>
+      </c>
+      <c r="J1195">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1196" spans="6:10">
+      <c r="F1196">
+        <v>15275</v>
+      </c>
+      <c r="J1196">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1197" spans="6:10">
+      <c r="F1197">
+        <v>15288</v>
+      </c>
+      <c r="J1197">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1198" spans="6:10">
+      <c r="F1198">
+        <v>15301</v>
+      </c>
+      <c r="J1198">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1199" spans="6:10">
+      <c r="F1199">
+        <v>15314</v>
+      </c>
+      <c r="J1199">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1200" spans="6:10">
+      <c r="F1200">
+        <v>15326</v>
+      </c>
+      <c r="J1200">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1201" spans="6:10">
+      <c r="F1201">
+        <v>15339</v>
+      </c>
+      <c r="J1201">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1202" spans="6:10">
+      <c r="F1202">
+        <v>15352</v>
+      </c>
+      <c r="J1202">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1203" spans="6:10">
+      <c r="F1203">
+        <v>15365</v>
+      </c>
+      <c r="J1203">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1204" spans="6:10">
+      <c r="F1204">
+        <v>15378</v>
+      </c>
+      <c r="J1204">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1205" spans="6:10">
+      <c r="F1205">
+        <v>15390</v>
+      </c>
+      <c r="J1205">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1206" spans="6:10">
+      <c r="F1206">
+        <v>15403</v>
+      </c>
+      <c r="J1206">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1207" spans="6:10">
+      <c r="F1207">
+        <v>15416</v>
+      </c>
+      <c r="J1207">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1208" spans="6:10">
+      <c r="F1208">
+        <v>15429</v>
+      </c>
+      <c r="J1208">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1209" spans="6:10">
+      <c r="F1209">
+        <v>15442</v>
+      </c>
+      <c r="J1209">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1210" spans="6:10">
+      <c r="F1210">
+        <v>15454</v>
+      </c>
+      <c r="J1210">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1211" spans="6:10">
+      <c r="F1211">
+        <v>15467</v>
+      </c>
+      <c r="J1211">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1212" spans="6:10">
+      <c r="F1212">
+        <v>15480</v>
+      </c>
+      <c r="J1212">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1213" spans="6:10">
+      <c r="F1213">
+        <v>15493</v>
+      </c>
+      <c r="J1213">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1214" spans="6:10">
+      <c r="F1214">
+        <v>15506</v>
+      </c>
+      <c r="J1214">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1215" spans="6:10">
+      <c r="F1215">
+        <v>15518</v>
+      </c>
+      <c r="J1215">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1216" spans="6:10">
+      <c r="F1216">
+        <v>15531</v>
+      </c>
+      <c r="J1216">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1217" spans="6:10">
+      <c r="F1217">
+        <v>15544</v>
+      </c>
+      <c r="J1217">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1218" spans="6:10">
+      <c r="F1218">
+        <v>15557</v>
+      </c>
+      <c r="J1218">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1219" spans="6:10">
+      <c r="F1219">
+        <v>15570</v>
+      </c>
+      <c r="J1219">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1220" spans="6:10">
+      <c r="F1220">
+        <v>15582</v>
+      </c>
+      <c r="J1220">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1221" spans="6:10">
+      <c r="F1221">
+        <v>15595</v>
+      </c>
+      <c r="J1221">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1222" spans="6:10">
+      <c r="F1222">
+        <v>15608</v>
+      </c>
+      <c r="J1222">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1223" spans="6:10">
+      <c r="F1223">
+        <v>15621</v>
+      </c>
+      <c r="J1223">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1224" spans="6:10">
+      <c r="F1224">
+        <v>15634</v>
+      </c>
+      <c r="J1224">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1225" spans="6:10">
+      <c r="F1225">
+        <v>15646</v>
+      </c>
+      <c r="J1225">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1226" spans="6:10">
+      <c r="F1226">
+        <v>15659</v>
+      </c>
+      <c r="J1226">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1227" spans="6:10">
+      <c r="F1227">
+        <v>15672</v>
+      </c>
+      <c r="J1227">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1228" spans="6:10">
+      <c r="F1228">
+        <v>15685</v>
+      </c>
+      <c r="J1228">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1229" spans="6:10">
+      <c r="F1229">
+        <v>15698</v>
+      </c>
+      <c r="J1229">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1230" spans="6:10">
+      <c r="F1230">
+        <v>15710</v>
+      </c>
+      <c r="J1230">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1231" spans="6:10">
+      <c r="F1231">
+        <v>15723</v>
+      </c>
+      <c r="J1231">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1232" spans="6:10">
+      <c r="F1232">
+        <v>15736</v>
+      </c>
+      <c r="J1232">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1233" spans="6:10">
+      <c r="F1233">
+        <v>15749</v>
+      </c>
+      <c r="J1233">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1234" spans="6:10">
+      <c r="F1234">
+        <v>15762</v>
+      </c>
+      <c r="J1234">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1235" spans="6:10">
+      <c r="F1235">
+        <v>15774</v>
+      </c>
+      <c r="J1235">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1236" spans="6:10">
+      <c r="F1236">
+        <v>15787</v>
+      </c>
+      <c r="J1236">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1237" spans="6:10">
+      <c r="F1237">
+        <v>15800</v>
+      </c>
+      <c r="J1237">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1238" spans="6:10">
+      <c r="F1238">
+        <v>15813</v>
+      </c>
+      <c r="J1238">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1239" spans="6:10">
+      <c r="F1239">
+        <v>15826</v>
+      </c>
+      <c r="J1239">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1240" spans="6:10">
+      <c r="F1240">
+        <v>15838</v>
+      </c>
+      <c r="J1240">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1241" spans="6:10">
+      <c r="F1241">
+        <v>15851</v>
+      </c>
+      <c r="J1241">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1242" spans="6:10">
+      <c r="F1242">
+        <v>15864</v>
+      </c>
+      <c r="J1242">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1243" spans="6:10">
+      <c r="F1243">
+        <v>15877</v>
+      </c>
+      <c r="J1243">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1244" spans="6:10">
+      <c r="F1244">
+        <v>15890</v>
+      </c>
+      <c r="J1244">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1245" spans="6:10">
+      <c r="F1245">
+        <v>15902</v>
+      </c>
+      <c r="J1245">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1246" spans="6:10">
+      <c r="F1246">
+        <v>15915</v>
+      </c>
+      <c r="J1246">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1247" spans="6:10">
+      <c r="F1247">
+        <v>15928</v>
+      </c>
+      <c r="J1247">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1248" spans="6:10">
+      <c r="F1248">
+        <v>15941</v>
+      </c>
+      <c r="J1248">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1249" spans="6:10">
+      <c r="F1249">
+        <v>15954</v>
+      </c>
+      <c r="J1249">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1250" spans="6:10">
+      <c r="F1250">
+        <v>15966</v>
+      </c>
+      <c r="J1250">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1251" spans="6:10">
+      <c r="F1251">
+        <v>15979</v>
+      </c>
+      <c r="J1251">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1252" spans="6:10">
+      <c r="F1252">
+        <v>15992</v>
+      </c>
+      <c r="J1252">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1253" spans="6:10">
+      <c r="F1253">
+        <v>16005</v>
+      </c>
+      <c r="J1253">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1254" spans="6:10">
+      <c r="F1254">
+        <v>16018</v>
+      </c>
+      <c r="J1254">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1255" spans="6:10">
+      <c r="F1255">
+        <v>16030</v>
+      </c>
+      <c r="J1255">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1256" spans="6:10">
+      <c r="F1256">
+        <v>16043</v>
+      </c>
+      <c r="J1256">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1257" spans="6:10">
+      <c r="F1257">
+        <v>16056</v>
+      </c>
+      <c r="J1257">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1258" spans="6:10">
+      <c r="F1258">
+        <v>16069</v>
+      </c>
+      <c r="J1258">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1259" spans="6:10">
+      <c r="F1259">
+        <v>16082</v>
+      </c>
+      <c r="J1259">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1260" spans="6:10">
+      <c r="F1260">
+        <v>16094</v>
+      </c>
+      <c r="J1260">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1261" spans="6:10">
+      <c r="F1261">
+        <v>16107</v>
+      </c>
+      <c r="J1261">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1262" spans="6:10">
+      <c r="F1262">
+        <v>16120</v>
+      </c>
+      <c r="J1262">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1263" spans="6:10">
+      <c r="F1263">
+        <v>16133</v>
+      </c>
+      <c r="J1263">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1264" spans="6:10">
+      <c r="F1264">
+        <v>16146</v>
+      </c>
+      <c r="J1264">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1265" spans="6:10">
+      <c r="F1265">
+        <v>16158</v>
+      </c>
+      <c r="J1265">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1266" spans="6:10">
+      <c r="F1266">
+        <v>16171</v>
+      </c>
+      <c r="J1266">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1267" spans="6:10">
+      <c r="F1267">
+        <v>16184</v>
+      </c>
+      <c r="J1267">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1268" spans="6:10">
+      <c r="F1268">
+        <v>16197</v>
+      </c>
+      <c r="J1268">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1269" spans="6:10">
+      <c r="F1269">
+        <v>16210</v>
+      </c>
+      <c r="J1269">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1270" spans="6:10">
+      <c r="F1270">
+        <v>16222</v>
+      </c>
+      <c r="J1270">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1271" spans="6:10">
+      <c r="F1271">
+        <v>16235</v>
+      </c>
+      <c r="J1271">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1272" spans="6:10">
+      <c r="F1272">
+        <v>16248</v>
+      </c>
+      <c r="J1272">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1273" spans="6:10">
+      <c r="F1273">
+        <v>16261</v>
+      </c>
+      <c r="J1273">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1274" spans="6:10">
+      <c r="F1274">
+        <v>16274</v>
+      </c>
+      <c r="J1274">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1275" spans="6:10">
+      <c r="F1275">
+        <v>16286</v>
+      </c>
+      <c r="J1275">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1276" spans="6:10">
+      <c r="F1276">
+        <v>16299</v>
+      </c>
+      <c r="J1276">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1277" spans="6:10">
+      <c r="F1277">
+        <v>16312</v>
+      </c>
+      <c r="J1277">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1278" spans="6:10">
+      <c r="F1278">
+        <v>16325</v>
+      </c>
+      <c r="J1278">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1279" spans="6:10">
+      <c r="F1279">
+        <v>16338</v>
+      </c>
+      <c r="J1279">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1280" spans="6:10">
+      <c r="F1280">
+        <v>16350</v>
+      </c>
+      <c r="J1280">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1281" spans="6:10">
+      <c r="F1281">
+        <v>16363</v>
+      </c>
+      <c r="J1281">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1282" spans="6:10">
+      <c r="F1282">
+        <v>16376</v>
+      </c>
+      <c r="J1282">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1283" spans="6:10">
+      <c r="F1283">
+        <v>16389</v>
+      </c>
+      <c r="J1283">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1284" spans="6:10">
+      <c r="F1284">
+        <v>16402</v>
+      </c>
+      <c r="J1284">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1285" spans="6:10">
+      <c r="F1285">
+        <v>16414</v>
+      </c>
+      <c r="J1285">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1286" spans="6:10">
+      <c r="F1286">
+        <v>16427</v>
+      </c>
+      <c r="J1286">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1287" spans="6:10">
+      <c r="F1287">
+        <v>16440</v>
+      </c>
+      <c r="J1287">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1288" spans="6:10">
+      <c r="F1288">
+        <v>16453</v>
+      </c>
+      <c r="J1288">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1289" spans="6:10">
+      <c r="F1289">
+        <v>16466</v>
+      </c>
+      <c r="J1289">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1290" spans="6:10">
+      <c r="F1290">
+        <v>16478</v>
+      </c>
+      <c r="J1290">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1291" spans="6:10">
+      <c r="F1291">
+        <v>16491</v>
+      </c>
+      <c r="J1291">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1292" spans="6:10">
+      <c r="F1292">
+        <v>16504</v>
+      </c>
+      <c r="J1292">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1293" spans="6:10">
+      <c r="F1293">
+        <v>16517</v>
+      </c>
+      <c r="J1293">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1294" spans="6:10">
+      <c r="F1294">
+        <v>16530</v>
+      </c>
+      <c r="J1294">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1295" spans="6:10">
+      <c r="F1295">
+        <v>16542</v>
+      </c>
+      <c r="J1295">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1296" spans="6:10">
+      <c r="F1296">
+        <v>16555</v>
+      </c>
+      <c r="J1296">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1297" spans="6:10">
+      <c r="F1297">
+        <v>16568</v>
+      </c>
+      <c r="J1297">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1298" spans="6:10">
+      <c r="F1298">
+        <v>16581</v>
+      </c>
+      <c r="J1298">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1299" spans="6:10">
+      <c r="F1299">
+        <v>16594</v>
+      </c>
+      <c r="J1299">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1300" spans="6:10">
+      <c r="F1300">
+        <v>16606</v>
+      </c>
+      <c r="J1300">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1301" spans="6:10">
+      <c r="F1301">
+        <v>16619</v>
+      </c>
+      <c r="J1301">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1302" spans="6:10">
+      <c r="F1302">
+        <v>16632</v>
+      </c>
+      <c r="J1302">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1303" spans="6:10">
+      <c r="F1303">
+        <v>16645</v>
+      </c>
+      <c r="J1303">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1304" spans="6:10">
+      <c r="F1304">
+        <v>16658</v>
+      </c>
+      <c r="J1304">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1305" spans="6:10">
+      <c r="F1305">
+        <v>16670</v>
+      </c>
+      <c r="J1305">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1306" spans="6:10">
+      <c r="F1306">
+        <v>16683</v>
+      </c>
+      <c r="J1306">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1307" spans="6:10">
+      <c r="F1307">
+        <v>16696</v>
+      </c>
+      <c r="J1307">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1308" spans="6:10">
+      <c r="F1308">
+        <v>16709</v>
+      </c>
+      <c r="J1308">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1309" spans="6:10">
+      <c r="F1309">
+        <v>16722</v>
+      </c>
+      <c r="J1309">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1310" spans="6:10">
+      <c r="F1310">
+        <v>16734</v>
+      </c>
+      <c r="J1310">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1311" spans="6:10">
+      <c r="F1311">
+        <v>16747</v>
+      </c>
+      <c r="J1311">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1312" spans="6:10">
+      <c r="F1312">
+        <v>16760</v>
+      </c>
+      <c r="J1312">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1313" spans="6:10">
+      <c r="F1313">
+        <v>16773</v>
+      </c>
+      <c r="J1313">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1314" spans="6:10">
+      <c r="F1314">
+        <v>16786</v>
+      </c>
+      <c r="J1314">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1315" spans="6:10">
+      <c r="F1315">
+        <v>16798</v>
+      </c>
+      <c r="J1315">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1316" spans="6:10">
+      <c r="F1316">
+        <v>16811</v>
+      </c>
+      <c r="J1316">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1317" spans="6:10">
+      <c r="F1317">
+        <v>16824</v>
+      </c>
+      <c r="J1317">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1318" spans="6:10">
+      <c r="F1318">
+        <v>16837</v>
+      </c>
+      <c r="J1318">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1319" spans="6:10">
+      <c r="F1319">
+        <v>16850</v>
+      </c>
+      <c r="J1319">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1320" spans="6:10">
+      <c r="F1320">
+        <v>16862</v>
+      </c>
+      <c r="J1320">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1321" spans="6:10">
+      <c r="F1321">
+        <v>16875</v>
+      </c>
+      <c r="J1321">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1322" spans="6:10">
+      <c r="F1322">
+        <v>16888</v>
+      </c>
+      <c r="J1322">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1323" spans="6:10">
+      <c r="F1323">
+        <v>16901</v>
+      </c>
+      <c r="J1323">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1324" spans="6:10">
+      <c r="F1324">
+        <v>16914</v>
+      </c>
+      <c r="J1324">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1325" spans="6:10">
+      <c r="F1325">
+        <v>16926</v>
+      </c>
+      <c r="J1325">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1326" spans="6:10">
+      <c r="F1326">
+        <v>16939</v>
+      </c>
+      <c r="J1326">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1327" spans="6:10">
+      <c r="F1327">
+        <v>16952</v>
+      </c>
+      <c r="J1327">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1328" spans="6:10">
+      <c r="F1328">
+        <v>16965</v>
+      </c>
+      <c r="J1328">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1329" spans="6:10">
+      <c r="F1329">
+        <v>16978</v>
+      </c>
+      <c r="J1329">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1330" spans="6:10">
+      <c r="F1330">
+        <v>16990</v>
+      </c>
+      <c r="J1330">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="1331" spans="6:10">
+      <c r="F1331">
+        <v>17003</v>
+      </c>
+      <c r="J1331">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1332" spans="6:10">
+      <c r="F1332">
+        <v>17016</v>
+      </c>
+      <c r="J1332">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1333" spans="6:10">
+      <c r="F1333">
+        <v>17029</v>
+      </c>
+      <c r="J1333">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1334" spans="6:10">
+      <c r="F1334">
+        <v>17042</v>
+      </c>
+      <c r="J1334">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1335" spans="6:10">
+      <c r="F1335">
+        <v>17054</v>
+      </c>
+      <c r="J1335">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1336" spans="6:10">
+      <c r="F1336">
+        <v>17067</v>
+      </c>
+      <c r="J1336">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1337" spans="6:10">
+      <c r="F1337">
+        <v>17080</v>
+      </c>
+      <c r="J1337">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1338" spans="6:10">
+      <c r="F1338">
+        <v>17093</v>
+      </c>
+      <c r="J1338">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1339" spans="6:10">
+      <c r="F1339">
+        <v>17106</v>
+      </c>
+      <c r="J1339">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1340" spans="6:10">
+      <c r="F1340">
+        <v>17118</v>
+      </c>
+      <c r="J1340">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1341" spans="6:10">
+      <c r="F1341">
+        <v>17131</v>
+      </c>
+      <c r="J1341">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1342" spans="6:10">
+      <c r="F1342">
+        <v>17144</v>
+      </c>
+      <c r="J1342">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1343" spans="6:10">
+      <c r="F1343">
+        <v>17157</v>
+      </c>
+      <c r="J1343">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1344" spans="6:10">
+      <c r="F1344">
+        <v>17170</v>
+      </c>
+      <c r="J1344">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1345" spans="6:10">
+      <c r="F1345">
+        <v>17182</v>
+      </c>
+      <c r="J1345">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1346" spans="6:10">
+      <c r="F1346">
+        <v>17195</v>
+      </c>
+      <c r="J1346">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1347" spans="6:10">
+      <c r="F1347">
+        <v>17208</v>
+      </c>
+      <c r="J1347">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1348" spans="6:10">
+      <c r="F1348">
+        <v>17221</v>
+      </c>
+      <c r="J1348">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="1349" spans="6:10">
+      <c r="F1349">
+        <v>17234</v>
+      </c>
+      <c r="J1349">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="1350" spans="6:10">
+      <c r="F1350">
+        <v>17246</v>
+      </c>
+      <c r="J1350">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="1351" spans="6:10">
+      <c r="F1351">
+        <v>17259</v>
+      </c>
+      <c r="J1351">
+        <v>2.4E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>